<commit_message>
Scaled up a crap ton
Can now input teams and get any team's (all 5 starters) odds to compare against sportsbook.

proposed odds located in bet_stamps.csv
</commit_message>
<xml_diff>
--- a/Bet Stamps.xlsx
+++ b/Bet Stamps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsham\.spyder-py3\beating-the-books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831126D4-B7F6-473E-B309-E66CCA7046EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE03AE0-6C28-4133-A0AA-EC6336F13FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,30 @@
   </si>
   <si>
     <t>Tatum 25+PTS</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Garland 4+ reb</t>
+  </si>
+  <si>
+    <t>Garland 10+ pts</t>
+  </si>
+  <si>
+    <t>mobley 10+ pts</t>
+  </si>
+  <si>
+    <t>strus 10+ pts</t>
+  </si>
+  <si>
+    <t>KCP 10+ pts</t>
+  </si>
+  <si>
+    <t>Gordon 10+ pts</t>
   </si>
 </sst>
 </file>
@@ -394,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1.06</v>
@@ -453,6 +477,13 @@
         <f>E2/D2-1</f>
         <v>0.1132075471698113</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <f>IF(G2="Yes",E2*C2-C2,-C2)</f>
+        <v>0.89999999999999947</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -473,6 +504,139 @@
       <c r="F3" s="2">
         <f>E3/D3-1</f>
         <v>0.25174825174825188</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <f>IF(G3="Yes",E3*C3-C3,-C3)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2.71</v>
+      </c>
+      <c r="E4">
+        <v>3.6</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F9" si="0">E4/D4-1</f>
+        <v>0.32841328413284132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1.02</v>
+      </c>
+      <c r="E5">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8039215686274606E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1.03</v>
+      </c>
+      <c r="E6">
+        <v>1.24</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20388349514563098</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1.25</v>
+      </c>
+      <c r="E7">
+        <v>1.83</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.46399999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1.6</v>
+      </c>
+      <c r="E8">
+        <v>2.35</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1.08</v>
+      </c>
+      <c r="E9">
+        <v>1.23</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13888888888888884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some starting lineups
</commit_message>
<xml_diff>
--- a/Bet Stamps.xlsx
+++ b/Bet Stamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsham\.spyder-py3\beating-the-books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE03AE0-6C28-4133-A0AA-EC6336F13FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60746B3B-5A71-4D15-A273-99B275656BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,42 @@
   </si>
   <si>
     <t>Gordon 10+ pts</t>
+  </si>
+  <si>
+    <t>Kawhi 20+ pts</t>
+  </si>
+  <si>
+    <t>Austin Reeves 15+ pts</t>
+  </si>
+  <si>
+    <t>Rui Hachimura 4+ rebs</t>
+  </si>
+  <si>
+    <t>Lebron 20+ pts</t>
+  </si>
+  <si>
+    <t>D'angelo Russel 6+ assits</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Nic Claxton</t>
+  </si>
+  <si>
+    <t>Mikal Bridges</t>
+  </si>
+  <si>
+    <t>10+ pts</t>
+  </si>
+  <si>
+    <t>15+ pts</t>
+  </si>
+  <si>
+    <t>6+ rebs</t>
+  </si>
+  <si>
+    <t>Terry Rozier</t>
   </si>
 </sst>
 </file>
@@ -418,225 +454,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45381</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.06</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.18</v>
       </c>
-      <c r="F2" s="2">
-        <f>E2/D2-1</f>
+      <c r="G2" s="2">
+        <f>F2/E2-1</f>
         <v>0.1132075471698113</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2">
-        <f>IF(G2="Yes",E2*C2-C2,-C2)</f>
+      <c r="I2">
+        <f>IF(H2="Yes",F2*D2-D2,-D2)</f>
         <v>0.89999999999999947</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45381</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>1.43</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1.79</v>
       </c>
-      <c r="F3" s="2">
-        <f>E3/D3-1</f>
+      <c r="G3" s="2">
+        <f>F3/E3-1</f>
         <v>0.25174825174825188</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3">
-        <f>IF(G3="Yes",E3*C3-C3,-C3)</f>
+      <c r="I3">
+        <f>IF(H3="Yes",F3*D3-D3,-D3)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45382</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>2.71</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3.6</v>
       </c>
-      <c r="F4" s="2">
-        <f t="shared" ref="F4:F9" si="0">E4/D4-1</f>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G18" si="0">F4/E4-1</f>
         <v>0.32841328413284132</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45382</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>1.02</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1.1200000000000001</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>9.8039215686274606E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45382</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>1.03</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1.24</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0.20388349514563098</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45382</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>1.25</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1.83</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0.46399999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45382</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>1.6</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2.35</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>0.46875</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45382</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>1.08</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>1.23</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>0.13888888888888884</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F10">
+        <v>1.4</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22807017543859653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1.48</v>
+      </c>
+      <c r="F11">
+        <v>1.74</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.17567567567567566</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1.5</v>
+      </c>
+      <c r="F12">
+        <v>1.71</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F13">
+        <v>1.3</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1711711711711712</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1.42</v>
+      </c>
+      <c r="F14">
+        <v>2.1</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.47887323943661975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1.34</v>
+      </c>
+      <c r="F15">
+        <v>1.51</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12686567164179108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1.04</v>
+      </c>
+      <c r="F16">
+        <v>1.32</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26923076923076916</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2.57</v>
+      </c>
+      <c r="F17">
+        <v>3.3</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28404669260700399</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1.06</v>
+      </c>
+      <c r="F18">
+        <v>1.56</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.47169811320754707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched Poisson to Normal Distribution
Also updated lineups and bet stamps
</commit_message>
<xml_diff>
--- a/Bet Stamps.xlsx
+++ b/Bet Stamps.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsham\.spyder-py3\beating-the-books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60746B3B-5A71-4D15-A273-99B275656BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A59BCCF-7828-42AD-93AC-03EE2DCDAED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -50,9 +53,6 @@
     <t>Net Result</t>
   </si>
   <si>
-    <t>Tatum 20+ PTs</t>
-  </si>
-  <si>
     <t>Calculated Exp Payout</t>
   </si>
   <si>
@@ -65,48 +65,12 @@
     <t>Hit?</t>
   </si>
   <si>
-    <t>Tatum 25+PTS</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>Garland 4+ reb</t>
-  </si>
-  <si>
-    <t>Garland 10+ pts</t>
-  </si>
-  <si>
-    <t>mobley 10+ pts</t>
-  </si>
-  <si>
-    <t>strus 10+ pts</t>
-  </si>
-  <si>
-    <t>KCP 10+ pts</t>
-  </si>
-  <si>
-    <t>Gordon 10+ pts</t>
-  </si>
-  <si>
-    <t>Kawhi 20+ pts</t>
-  </si>
-  <si>
-    <t>Austin Reeves 15+ pts</t>
-  </si>
-  <si>
-    <t>Rui Hachimura 4+ rebs</t>
-  </si>
-  <si>
-    <t>Lebron 20+ pts</t>
-  </si>
-  <si>
-    <t>D'angelo Russel 6+ assits</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -126,12 +90,120 @@
   </si>
   <si>
     <t>Terry Rozier</t>
+  </si>
+  <si>
+    <t>nikola vucevic</t>
+  </si>
+  <si>
+    <t>coby white</t>
+  </si>
+  <si>
+    <t>4+ asts</t>
+  </si>
+  <si>
+    <t>2+ asts</t>
+  </si>
+  <si>
+    <t>dillon brooks</t>
+  </si>
+  <si>
+    <t>chet holmgren</t>
+  </si>
+  <si>
+    <t>jalen williams</t>
+  </si>
+  <si>
+    <t>20+ pts</t>
+  </si>
+  <si>
+    <t>6+ asts</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>4+ rebs</t>
+  </si>
+  <si>
+    <t>25+ pts</t>
+  </si>
+  <si>
+    <t>6+ assists</t>
+  </si>
+  <si>
+    <t>D'angelo Russel</t>
+  </si>
+  <si>
+    <t>Tatum</t>
+  </si>
+  <si>
+    <t>Garland</t>
+  </si>
+  <si>
+    <t>mobley</t>
+  </si>
+  <si>
+    <t>strus</t>
+  </si>
+  <si>
+    <t>KCP</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>Kawhi</t>
+  </si>
+  <si>
+    <t>Austin Reeves</t>
+  </si>
+  <si>
+    <t>Rui Hachimura</t>
+  </si>
+  <si>
+    <t>Lebron</t>
+  </si>
+  <si>
+    <t>jrue holiday</t>
+  </si>
+  <si>
+    <t>Miles bridges</t>
+  </si>
+  <si>
+    <t>Myles Turner</t>
+  </si>
+  <si>
+    <t>Andrew Nembhard</t>
+  </si>
+  <si>
+    <t>Pascal Siakam</t>
+  </si>
+  <si>
+    <t>Santi Aldama</t>
+  </si>
+  <si>
+    <t>Jalen Suggs</t>
+  </si>
+  <si>
+    <t>Bradley Beal</t>
+  </si>
+  <si>
+    <t>Kevin Durant</t>
+  </si>
+  <si>
+    <t>Grayson Allen</t>
+  </si>
+  <si>
+    <t>Jusuf Nurkic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,12 +220,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,10 +253,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,31 +558,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -504,7 +591,10 @@
         <v>45381</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -520,7 +610,7 @@
         <v>0.1132075471698113</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I2">
         <f>IF(H2="Yes",F2*D2-D2,-D2)</f>
@@ -532,7 +622,10 @@
         <v>45381</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -548,7 +641,7 @@
         <v>0.25174825174825188</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I3">
         <f>IF(H3="Yes",F3*D3-D3,-D3)</f>
@@ -560,7 +653,10 @@
         <v>45382</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -572,8 +668,15 @@
         <v>3.6</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G18" si="0">F4/E4-1</f>
+        <f t="shared" ref="G4:G41" si="0">F4/E4-1</f>
         <v>0.32841328413284132</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I41" si="1">IF(H4="Yes",F4*D4-D4,-D4)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -581,6 +684,9 @@
         <v>45382</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5">
@@ -596,16 +702,26 @@
         <f t="shared" si="0"/>
         <v>9.8039215686274606E-2</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45382</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>1.03</v>
@@ -617,13 +733,23 @@
         <f t="shared" si="0"/>
         <v>0.20388349514563098</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45382</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -638,13 +764,23 @@
         <f t="shared" si="0"/>
         <v>0.46399999999999997</v>
       </c>
+      <c r="H7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45382</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -659,13 +795,23 @@
         <f t="shared" si="0"/>
         <v>0.46875</v>
       </c>
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1.35</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45382</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -680,13 +826,23 @@
         <f t="shared" si="0"/>
         <v>0.13888888888888884</v>
       </c>
+      <c r="H9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.22999999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45382</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -701,10 +857,23 @@
         <f t="shared" si="0"/>
         <v>0.22807017543859653</v>
       </c>
+      <c r="H10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.39999999999999991</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45382</v>
+      </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -719,10 +888,23 @@
         <f t="shared" si="0"/>
         <v>0.17567567567567566</v>
       </c>
+      <c r="H11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45382</v>
+      </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -737,10 +919,23 @@
         <f t="shared" si="0"/>
         <v>0.1399999999999999</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0.71</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45382</v>
+      </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -755,10 +950,23 @@
         <f t="shared" si="0"/>
         <v>0.1711711711711712</v>
       </c>
+      <c r="H13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45382</v>
+      </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -773,13 +981,23 @@
         <f t="shared" si="0"/>
         <v>0.47887323943661975</v>
       </c>
+      <c r="H14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45382</v>
+      </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -794,13 +1012,23 @@
         <f t="shared" si="0"/>
         <v>0.12686567164179108</v>
       </c>
+      <c r="H15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.51</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45382</v>
+      </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -815,13 +1043,23 @@
         <f t="shared" si="0"/>
         <v>0.26923076923076916</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45382</v>
+      </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -836,13 +1074,23 @@
         <f t="shared" si="0"/>
         <v>0.28404669260700399</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45382</v>
+      </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -857,8 +1105,748 @@
         <f t="shared" si="0"/>
         <v>0.47169811320754707</v>
       </c>
+      <c r="H18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1.22</v>
+      </c>
+      <c r="F19">
+        <v>1.77</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.45081967213114749</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F20">
+        <v>1.31</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18018018018018012</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0.31000000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="F21">
+        <v>3.3</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.59420289855072461</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F22">
+        <v>1.31</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13913043478260878</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0.31000000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1.25</v>
+      </c>
+      <c r="F23">
+        <v>1.45</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15999999999999992</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1.03</v>
+      </c>
+      <c r="F24">
+        <v>1.17</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13592233009708732</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1.43</v>
+      </c>
+      <c r="F26">
+        <v>1.74</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21678321678321688</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F27">
+        <v>1.43</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23275862068965525</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F28">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21890547263681603</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1.39</v>
+      </c>
+      <c r="F29">
+        <v>1.71</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23021582733812962</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1.02</v>
+      </c>
+      <c r="F30">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12745098039215685</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1.39</v>
+      </c>
+      <c r="F31">
+        <v>1.77</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27338129496402885</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1.7</v>
+      </c>
+      <c r="F32">
+        <v>1.95</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14705882352941169</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1.52</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.31578947368421062</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1.45</v>
+      </c>
+      <c r="F34">
+        <v>1.77</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22068965517241379</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F35">
+        <v>1.43</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26548672566371678</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>0.42999999999999994</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>2.41</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24481327800829877</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1.26</v>
+      </c>
+      <c r="F37">
+        <v>1.61</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2777777777777779</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1.08</v>
+      </c>
+      <c r="F38">
+        <v>1.24</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1.8</v>
+      </c>
+      <c r="F39">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333339</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1.3</v>
+      </c>
+      <c r="F40">
+        <v>1.59</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22307692307692317</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1.75</v>
+      </c>
+      <c r="F41">
+        <v>2.25</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28571428571428581</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f>SUM(D2:D49)</f>
+        <v>45</v>
+      </c>
+      <c r="I50">
+        <f>SUM(I2:I49)+D50</f>
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="3">
+        <f>I50/D50-1</f>
+        <v>-5.3333333333333344E-2</v>
+      </c>
+      <c r="J51" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying to fix nan bug
updated bet stamps
</commit_message>
<xml_diff>
--- a/Bet Stamps.xlsx
+++ b/Bet Stamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsham\.spyder-py3\beating-the-books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A59BCCF-7828-42AD-93AC-03EE2DCDAED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7020D3F-C182-418B-AF25-A9DB44B45288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,48 @@
   </si>
   <si>
     <t>Jusuf Nurkic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PJ washington </t>
+  </si>
+  <si>
+    <t>Derrick Jones Jr</t>
+  </si>
+  <si>
+    <t>2+ 3's</t>
+  </si>
+  <si>
+    <t>Derrick White</t>
+  </si>
+  <si>
+    <t>2+ 3s</t>
+  </si>
+  <si>
+    <t>Brook Lopez</t>
+  </si>
+  <si>
+    <t>Khris Middleton</t>
+  </si>
+  <si>
+    <t>Damian Lillard</t>
+  </si>
+  <si>
+    <t>Alex Caruso</t>
+  </si>
+  <si>
+    <t>Coby White</t>
+  </si>
+  <si>
+    <t>Jamal Murray</t>
+  </si>
+  <si>
+    <t>Stephen Curry</t>
+  </si>
+  <si>
+    <t>Kris Murray</t>
+  </si>
+  <si>
+    <t>day over day % change</t>
   </si>
 </sst>
 </file>
@@ -541,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,9 +597,10 @@
     <col min="4" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="8" width="16.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -585,8 +628,11 @@
       <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45381</v>
       </c>
@@ -616,8 +662,12 @@
         <f>IF(H2="Yes",F2*D2-D2,-D2)</f>
         <v>0.89999999999999947</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="str">
+        <f>IF(NOT(A2=A3),(SUMIFS(I:I, A:A, A2)+SUMIFS(D:D, A:A, A2))/SUMIFS(D:D, A:A, A2)-1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45381</v>
       </c>
@@ -647,8 +697,12 @@
         <f>IF(H3="Yes",F3*D3-D3,-D3)</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <f>IF(NOT(A3=A4),(SUMIFS(I:I, A:A, A3)+SUMIFS(D:D, A:A, A3))/SUMIFS(D:D, A:A, A3)-1,"")</f>
+        <v>-1.6666666666666718E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45382</v>
       </c>
@@ -668,18 +722,22 @@
         <v>3.6</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G41" si="0">F4/E4-1</f>
+        <f t="shared" ref="G4:G69" si="0">F4/E4-1</f>
         <v>0.32841328413284132</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I41" si="1">IF(H4="Yes",F4*D4-D4,-D4)</f>
+        <f t="shared" ref="I4:I67" si="1">IF(H4="Yes",F4*D4-D4,-D4)</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="str">
+        <f t="shared" ref="J4:J67" si="2">IF(NOT(A4=A5),(SUMIFS(I:I, A:A, A4)+SUMIFS(D:D, A:A, A4))/SUMIFS(D:D, A:A, A4)-1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45382</v>
       </c>
@@ -709,8 +767,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45382</v>
       </c>
@@ -740,8 +802,12 @@
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45382</v>
       </c>
@@ -771,8 +837,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45382</v>
       </c>
@@ -802,8 +872,12 @@
         <f t="shared" si="1"/>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45382</v>
       </c>
@@ -833,8 +907,12 @@
         <f t="shared" si="1"/>
         <v>0.22999999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45382</v>
       </c>
@@ -864,8 +942,12 @@
         <f t="shared" si="1"/>
         <v>0.39999999999999991</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45382</v>
       </c>
@@ -895,8 +977,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45382</v>
       </c>
@@ -926,8 +1012,12 @@
         <f t="shared" si="1"/>
         <v>0.71</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45382</v>
       </c>
@@ -957,8 +1047,12 @@
         <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45382</v>
       </c>
@@ -988,8 +1082,12 @@
         <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45382</v>
       </c>
@@ -1019,8 +1117,12 @@
         <f t="shared" si="1"/>
         <v>0.51</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45382</v>
       </c>
@@ -1050,8 +1152,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45382</v>
       </c>
@@ -1081,8 +1187,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45382</v>
       </c>
@@ -1112,8 +1222,12 @@
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45382</v>
       </c>
@@ -1143,8 +1257,12 @@
         <f t="shared" si="1"/>
         <v>0.77</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45382</v>
       </c>
@@ -1174,8 +1292,12 @@
         <f t="shared" si="1"/>
         <v>0.31000000000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45382</v>
       </c>
@@ -1205,8 +1327,12 @@
         <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45382</v>
       </c>
@@ -1236,8 +1362,12 @@
         <f t="shared" si="1"/>
         <v>0.31000000000000005</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45382</v>
       </c>
@@ -1267,8 +1397,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45382</v>
       </c>
@@ -1298,8 +1432,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45382</v>
       </c>
@@ -1329,8 +1467,12 @@
         <f t="shared" si="1"/>
         <v>1.2999999999999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45382</v>
       </c>
@@ -1360,8 +1502,12 @@
         <f t="shared" si="1"/>
         <v>0.74</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14041666666666663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45383</v>
       </c>
@@ -1391,8 +1537,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45383</v>
       </c>
@@ -1422,8 +1572,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45383</v>
       </c>
@@ -1453,8 +1607,12 @@
         <f t="shared" si="1"/>
         <v>0.71</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45383</v>
       </c>
@@ -1484,8 +1642,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45383</v>
       </c>
@@ -1515,8 +1677,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45383</v>
       </c>
@@ -1546,8 +1712,12 @@
         <f t="shared" si="1"/>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45383</v>
       </c>
@@ -1577,8 +1747,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45383</v>
       </c>
@@ -1608,8 +1782,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45383</v>
       </c>
@@ -1639,8 +1817,12 @@
         <f t="shared" si="1"/>
         <v>0.42999999999999994</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45383</v>
       </c>
@@ -1670,8 +1852,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45383</v>
       </c>
@@ -1701,8 +1887,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45383</v>
       </c>
@@ -1732,8 +1922,12 @@
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45383</v>
       </c>
@@ -1763,8 +1957,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45383</v>
       </c>
@@ -1794,8 +1992,12 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45383</v>
       </c>
@@ -1825,28 +2027,1026 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.378</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1.79</v>
+      </c>
+      <c r="F42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22905027932960897</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J42" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1.72</v>
+      </c>
+      <c r="F43">
+        <v>4.8</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7906976744186047</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J43" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1.6</v>
+      </c>
+      <c r="F44">
+        <v>1.91</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19374999999999987</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J44" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1.42</v>
+      </c>
+      <c r="F45">
+        <v>1.63</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="0"/>
+        <v>0.147887323943662</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="J45" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1.53</v>
+      </c>
+      <c r="F46">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33986928104575154</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="J46" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1.39</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="0"/>
+        <v>0.43884892086330951</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J47" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1.7</v>
+      </c>
+      <c r="F48">
+        <v>2.25</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="0"/>
+        <v>0.32352941176470584</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J48" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1.25</v>
+      </c>
+      <c r="F49">
+        <v>1.57</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="J49" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>27</v>
+      </c>
       <c r="D50">
-        <f>SUM(D2:D49)</f>
-        <v>45</v>
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F50">
+        <v>1.63</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="0"/>
+        <v>0.42982456140350878</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="I50">
-        <f>SUM(I2:I49)+D50</f>
-        <v>42.6</v>
-      </c>
-    </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="I51" s="3">
-        <f>I50/D50-1</f>
-        <v>-5.3333333333333344E-2</v>
-      </c>
-      <c r="J51" t="s">
+        <f t="shared" si="1"/>
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="J50" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1.37</v>
+      </c>
+      <c r="F51">
+        <v>1.8</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.31386861313868608</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="J51" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1.24</v>
+      </c>
+      <c r="F52">
+        <v>1.69</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="0"/>
+        <v>0.36290322580645151</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>0.69</v>
+      </c>
+      <c r="J52" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1.33</v>
+      </c>
+      <c r="F53">
+        <v>1.74</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.30827067669172914</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>0.74</v>
+      </c>
+      <c r="J53" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>2.15</v>
+      </c>
+      <c r="F54">
+        <v>4.7</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1860465116279073</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>3.7</v>
+      </c>
+      <c r="J54" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1.32</v>
+      </c>
+      <c r="F55">
+        <v>1.63</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23484848484848464</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="J55" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1.23</v>
+      </c>
+      <c r="F56">
+        <v>1.67</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="0"/>
+        <v>0.35772357723577231</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J56" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1.19</v>
+      </c>
+      <c r="F57">
+        <v>1.48</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24369747899159666</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+      <c r="J57" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1.82</v>
+      </c>
+      <c r="F58">
+        <v>3.3</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="0"/>
+        <v>0.81318681318681296</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="1"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J58" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1.23</v>
+      </c>
+      <c r="F59">
+        <v>1.48</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20325203252032531</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+      <c r="J59" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1.26</v>
+      </c>
+      <c r="F60">
+        <v>1.48</v>
+      </c>
+      <c r="G60" s="2">
+        <f t="shared" si="0"/>
+        <v>0.17460317460317465</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+      <c r="J60" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1.86</v>
+      </c>
+      <c r="F61">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G61" s="2">
+        <f t="shared" si="0"/>
+        <v>0.37096774193548376</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J61" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1.25</v>
+      </c>
+      <c r="F62">
+        <v>1.5</v>
+      </c>
+      <c r="G62" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J62" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1.19</v>
+      </c>
+      <c r="F63">
+        <v>1.77</v>
+      </c>
+      <c r="G63" s="2">
+        <f t="shared" si="0"/>
+        <v>0.48739495798319332</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="1"/>
+        <v>0.77</v>
+      </c>
+      <c r="J63" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1.47</v>
+      </c>
+      <c r="F64">
+        <v>1.95</v>
+      </c>
+      <c r="G64" s="2">
+        <f t="shared" si="0"/>
+        <v>0.32653061224489788</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J64" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1.37</v>
+      </c>
+      <c r="F65">
+        <v>1.63</v>
+      </c>
+      <c r="G65" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18978102189780999</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="1"/>
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="J65" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1.56</v>
+      </c>
+      <c r="F66">
+        <v>1.8</v>
+      </c>
+      <c r="G66" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15384615384615374</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J66" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1.5</v>
+      </c>
+      <c r="F67">
+        <v>1.8</v>
+      </c>
+      <c r="G67" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="J67" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" t="s">
+        <v>19</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1.24</v>
+      </c>
+      <c r="F68">
+        <v>1.45</v>
+      </c>
+      <c r="G68" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16935483870967749</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I68">
+        <f t="shared" ref="I68:I69" si="3">IF(H68="Yes",F68*D68-D68,-D68)</f>
+        <v>-1</v>
+      </c>
+      <c r="J68" s="2" t="str">
+        <f t="shared" ref="J68:J69" si="4">IF(NOT(A68=A69),(SUMIFS(I:I, A:A, A68)+SUMIFS(D:D, A:A, A68))/SUMIFS(D:D, A:A, A68)-1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="F69">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G69" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18357487922705329</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="J69" s="2">
+        <f t="shared" si="4"/>
+        <v>0.17428571428571416</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>45392</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <f>SUM(D2:D79)</f>
+        <v>73</v>
+      </c>
+      <c r="I80">
+        <f>SUM(I2:I79)+D80</f>
+        <v>75.48</v>
+      </c>
+    </row>
+    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I81" s="3">
+        <f>I80/D80-1</f>
+        <v>3.3972602739726021E-2</v>
+      </c>
+      <c r="J81" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made records of all computed bet odds
Now stores all unique bets as a new csv file instead of replacing the existing one
</commit_message>
<xml_diff>
--- a/Bet Stamps.xlsx
+++ b/Bet Stamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsham\.spyder-py3\beating-the-books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7020D3F-C182-418B-AF25-A9DB44B45288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C08E1D-FCF2-4CE1-8BDB-6013399CCF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$109</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -237,6 +259,66 @@
   </si>
   <si>
     <t>day over day % change</t>
+  </si>
+  <si>
+    <t>Max Strus</t>
+  </si>
+  <si>
+    <t>Donovan Mitchell</t>
+  </si>
+  <si>
+    <t>evan Mobley</t>
+  </si>
+  <si>
+    <t>Tre Mann</t>
+  </si>
+  <si>
+    <t>Bam Adebayo</t>
+  </si>
+  <si>
+    <t>Tyler Herro</t>
+  </si>
+  <si>
+    <t>Kyrie Irving</t>
+  </si>
+  <si>
+    <t>Paolo Banchero</t>
+  </si>
+  <si>
+    <t>Wendell Carter Jr.</t>
+  </si>
+  <si>
+    <t>Franz Wagner</t>
+  </si>
+  <si>
+    <t>Mikal bridges</t>
+  </si>
+  <si>
+    <t>Dennis Schroder</t>
+  </si>
+  <si>
+    <t>SGA</t>
+  </si>
+  <si>
+    <t>kcp</t>
+  </si>
+  <si>
+    <t>Michael Porter Jr</t>
+  </si>
+  <si>
+    <t>Aaron Gordon</t>
+  </si>
+  <si>
+    <t>Mike Conley</t>
+  </si>
+  <si>
+    <t>Jaden McDanieels</t>
+  </si>
+  <si>
+    <t>Devin Booker</t>
+  </si>
+  <si>
+    <t>push</t>
   </si>
 </sst>
 </file>
@@ -583,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="G122" sqref="G122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +804,7 @@
         <v>3.6</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G69" si="0">F4/E4-1</f>
+        <f t="shared" ref="G4:G76" si="0">F4/E4-1</f>
         <v>0.32841328413284132</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -733,7 +815,7 @@
         <v>-1</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f t="shared" ref="J4:J67" si="2">IF(NOT(A4=A5),(SUMIFS(I:I, A:A, A4)+SUMIFS(D:D, A:A, A4))/SUMIFS(D:D, A:A, A4)-1,"")</f>
+        <f>IF(NOT(A4=A5),(SUMIFS(I:I, A:A, A4)+SUMIFS(D:D, A:A, A4))/SUMIFS(D:D, A:A, A4)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -768,7 +850,7 @@
         <v>-1</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A5=A6),(SUMIFS(I:I, A:A, A5)+SUMIFS(D:D, A:A, A5))/SUMIFS(D:D, A:A, A5)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -803,7 +885,7 @@
         <v>0.48</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A6=A7),(SUMIFS(I:I, A:A, A6)+SUMIFS(D:D, A:A, A6))/SUMIFS(D:D, A:A, A6)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -838,7 +920,7 @@
         <v>-1</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A7=A8),(SUMIFS(I:I, A:A, A7)+SUMIFS(D:D, A:A, A7))/SUMIFS(D:D, A:A, A7)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -873,7 +955,7 @@
         <v>1.35</v>
       </c>
       <c r="J8" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A8=A9),(SUMIFS(I:I, A:A, A8)+SUMIFS(D:D, A:A, A8))/SUMIFS(D:D, A:A, A8)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -908,7 +990,7 @@
         <v>0.22999999999999998</v>
       </c>
       <c r="J9" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A9=A10),(SUMIFS(I:I, A:A, A9)+SUMIFS(D:D, A:A, A9))/SUMIFS(D:D, A:A, A9)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -943,7 +1025,7 @@
         <v>0.39999999999999991</v>
       </c>
       <c r="J10" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A10=A11),(SUMIFS(I:I, A:A, A10)+SUMIFS(D:D, A:A, A10))/SUMIFS(D:D, A:A, A10)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -978,7 +1060,7 @@
         <v>-1</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A11=A12),(SUMIFS(I:I, A:A, A11)+SUMIFS(D:D, A:A, A11))/SUMIFS(D:D, A:A, A11)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1013,7 +1095,7 @@
         <v>0.71</v>
       </c>
       <c r="J12" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A12=A13),(SUMIFS(I:I, A:A, A12)+SUMIFS(D:D, A:A, A12))/SUMIFS(D:D, A:A, A12)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1048,7 +1130,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="J13" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A13=A14),(SUMIFS(I:I, A:A, A13)+SUMIFS(D:D, A:A, A13))/SUMIFS(D:D, A:A, A13)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1083,7 +1165,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A14=A15),(SUMIFS(I:I, A:A, A14)+SUMIFS(D:D, A:A, A14))/SUMIFS(D:D, A:A, A14)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1118,7 +1200,7 @@
         <v>0.51</v>
       </c>
       <c r="J15" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A15=A16),(SUMIFS(I:I, A:A, A15)+SUMIFS(D:D, A:A, A15))/SUMIFS(D:D, A:A, A15)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1153,7 +1235,7 @@
         <v>-1</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A16=A17),(SUMIFS(I:I, A:A, A16)+SUMIFS(D:D, A:A, A16))/SUMIFS(D:D, A:A, A16)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1188,7 +1270,7 @@
         <v>-1</v>
       </c>
       <c r="J17" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A17=A18),(SUMIFS(I:I, A:A, A17)+SUMIFS(D:D, A:A, A17))/SUMIFS(D:D, A:A, A17)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1223,7 +1305,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A18=A19),(SUMIFS(I:I, A:A, A18)+SUMIFS(D:D, A:A, A18))/SUMIFS(D:D, A:A, A18)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1258,7 +1340,7 @@
         <v>0.77</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A19=A20),(SUMIFS(I:I, A:A, A19)+SUMIFS(D:D, A:A, A19))/SUMIFS(D:D, A:A, A19)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1293,7 +1375,7 @@
         <v>0.31000000000000005</v>
       </c>
       <c r="J20" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A20=A21),(SUMIFS(I:I, A:A, A20)+SUMIFS(D:D, A:A, A20))/SUMIFS(D:D, A:A, A20)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1328,7 +1410,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A21=A22),(SUMIFS(I:I, A:A, A21)+SUMIFS(D:D, A:A, A21))/SUMIFS(D:D, A:A, A21)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1363,7 +1445,7 @@
         <v>0.31000000000000005</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A22=A23),(SUMIFS(I:I, A:A, A22)+SUMIFS(D:D, A:A, A22))/SUMIFS(D:D, A:A, A22)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1398,7 +1480,7 @@
         <v>-1</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A23=A24),(SUMIFS(I:I, A:A, A23)+SUMIFS(D:D, A:A, A23))/SUMIFS(D:D, A:A, A23)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1433,7 +1515,7 @@
         <v>-1</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A24=A25),(SUMIFS(I:I, A:A, A24)+SUMIFS(D:D, A:A, A24))/SUMIFS(D:D, A:A, A24)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1468,7 +1550,7 @@
         <v>1.2999999999999998</v>
       </c>
       <c r="J25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A25=A26),(SUMIFS(I:I, A:A, A25)+SUMIFS(D:D, A:A, A25))/SUMIFS(D:D, A:A, A25)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1503,7 +1585,7 @@
         <v>0.74</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A26=A27),(SUMIFS(I:I, A:A, A26)+SUMIFS(D:D, A:A, A26))/SUMIFS(D:D, A:A, A26)-1,"")</f>
         <v>0.14041666666666663</v>
       </c>
     </row>
@@ -1538,7 +1620,7 @@
         <v>-1</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A27=A28),(SUMIFS(I:I, A:A, A27)+SUMIFS(D:D, A:A, A27))/SUMIFS(D:D, A:A, A27)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1573,7 +1655,7 @@
         <v>-1</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A28=A29),(SUMIFS(I:I, A:A, A28)+SUMIFS(D:D, A:A, A28))/SUMIFS(D:D, A:A, A28)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1608,7 +1690,7 @@
         <v>0.71</v>
       </c>
       <c r="J29" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A29=A30),(SUMIFS(I:I, A:A, A29)+SUMIFS(D:D, A:A, A29))/SUMIFS(D:D, A:A, A29)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1643,7 +1725,7 @@
         <v>-1</v>
       </c>
       <c r="J30" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A30=A31),(SUMIFS(I:I, A:A, A30)+SUMIFS(D:D, A:A, A30))/SUMIFS(D:D, A:A, A30)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1678,7 +1760,7 @@
         <v>-1</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A31=A32),(SUMIFS(I:I, A:A, A31)+SUMIFS(D:D, A:A, A31))/SUMIFS(D:D, A:A, A31)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1713,7 +1795,7 @@
         <v>0.95</v>
       </c>
       <c r="J32" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A32=A33),(SUMIFS(I:I, A:A, A32)+SUMIFS(D:D, A:A, A32))/SUMIFS(D:D, A:A, A32)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1748,7 +1830,7 @@
         <v>-1</v>
       </c>
       <c r="J33" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A33=A34),(SUMIFS(I:I, A:A, A33)+SUMIFS(D:D, A:A, A33))/SUMIFS(D:D, A:A, A33)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1783,7 +1865,7 @@
         <v>-1</v>
       </c>
       <c r="J34" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A34=A35),(SUMIFS(I:I, A:A, A34)+SUMIFS(D:D, A:A, A34))/SUMIFS(D:D, A:A, A34)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1818,7 +1900,7 @@
         <v>0.42999999999999994</v>
       </c>
       <c r="J35" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A35=A36),(SUMIFS(I:I, A:A, A35)+SUMIFS(D:D, A:A, A35))/SUMIFS(D:D, A:A, A35)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1853,7 +1935,7 @@
         <v>2</v>
       </c>
       <c r="J36" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A36=A37),(SUMIFS(I:I, A:A, A36)+SUMIFS(D:D, A:A, A36))/SUMIFS(D:D, A:A, A36)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1888,7 +1970,7 @@
         <v>-1</v>
       </c>
       <c r="J37" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A37=A38),(SUMIFS(I:I, A:A, A37)+SUMIFS(D:D, A:A, A37))/SUMIFS(D:D, A:A, A37)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1923,7 +2005,7 @@
         <v>0.24</v>
       </c>
       <c r="J38" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A38=A39),(SUMIFS(I:I, A:A, A38)+SUMIFS(D:D, A:A, A38))/SUMIFS(D:D, A:A, A38)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1958,7 +2040,7 @@
         <v>-1</v>
       </c>
       <c r="J39" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A39=A40),(SUMIFS(I:I, A:A, A39)+SUMIFS(D:D, A:A, A39))/SUMIFS(D:D, A:A, A39)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -1993,7 +2075,7 @@
         <v>-1</v>
       </c>
       <c r="J40" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A40=A41),(SUMIFS(I:I, A:A, A40)+SUMIFS(D:D, A:A, A40))/SUMIFS(D:D, A:A, A40)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2028,7 +2110,7 @@
         <v>-1</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A41=A42),(SUMIFS(I:I, A:A, A41)+SUMIFS(D:D, A:A, A41))/SUMIFS(D:D, A:A, A41)-1,"")</f>
         <v>-0.378</v>
       </c>
     </row>
@@ -2063,7 +2145,7 @@
         <v>-1</v>
       </c>
       <c r="J42" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A42=A43),(SUMIFS(I:I, A:A, A42)+SUMIFS(D:D, A:A, A42))/SUMIFS(D:D, A:A, A42)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2098,7 +2180,7 @@
         <v>-1</v>
       </c>
       <c r="J43" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A43=A44),(SUMIFS(I:I, A:A, A43)+SUMIFS(D:D, A:A, A43))/SUMIFS(D:D, A:A, A43)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2133,7 +2215,7 @@
         <v>-1</v>
       </c>
       <c r="J44" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A44=A45),(SUMIFS(I:I, A:A, A44)+SUMIFS(D:D, A:A, A44))/SUMIFS(D:D, A:A, A44)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2168,7 +2250,7 @@
         <v>0.62999999999999989</v>
       </c>
       <c r="J45" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A45=A46),(SUMIFS(I:I, A:A, A45)+SUMIFS(D:D, A:A, A45))/SUMIFS(D:D, A:A, A45)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2203,7 +2285,7 @@
         <v>1.0499999999999998</v>
       </c>
       <c r="J46" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A46=A47),(SUMIFS(I:I, A:A, A46)+SUMIFS(D:D, A:A, A46))/SUMIFS(D:D, A:A, A46)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2238,7 +2320,7 @@
         <v>-1</v>
       </c>
       <c r="J47" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A47=A48),(SUMIFS(I:I, A:A, A47)+SUMIFS(D:D, A:A, A47))/SUMIFS(D:D, A:A, A47)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2273,7 +2355,7 @@
         <v>-1</v>
       </c>
       <c r="J48" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A48=A49),(SUMIFS(I:I, A:A, A48)+SUMIFS(D:D, A:A, A48))/SUMIFS(D:D, A:A, A48)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2308,7 +2390,7 @@
         <v>0.57000000000000006</v>
       </c>
       <c r="J49" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A49=A50),(SUMIFS(I:I, A:A, A49)+SUMIFS(D:D, A:A, A49))/SUMIFS(D:D, A:A, A49)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2343,7 +2425,7 @@
         <v>0.62999999999999989</v>
       </c>
       <c r="J50" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A50=A51),(SUMIFS(I:I, A:A, A50)+SUMIFS(D:D, A:A, A50))/SUMIFS(D:D, A:A, A50)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2378,7 +2460,7 @@
         <v>0.8</v>
       </c>
       <c r="J51" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A51=A52),(SUMIFS(I:I, A:A, A51)+SUMIFS(D:D, A:A, A51))/SUMIFS(D:D, A:A, A51)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2413,7 +2495,7 @@
         <v>0.69</v>
       </c>
       <c r="J52" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A52=A53),(SUMIFS(I:I, A:A, A52)+SUMIFS(D:D, A:A, A52))/SUMIFS(D:D, A:A, A52)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2448,7 +2530,7 @@
         <v>0.74</v>
       </c>
       <c r="J53" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A53=A54),(SUMIFS(I:I, A:A, A53)+SUMIFS(D:D, A:A, A53))/SUMIFS(D:D, A:A, A53)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2483,7 +2565,7 @@
         <v>3.7</v>
       </c>
       <c r="J54" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A54=A55),(SUMIFS(I:I, A:A, A54)+SUMIFS(D:D, A:A, A54))/SUMIFS(D:D, A:A, A54)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2518,7 +2600,7 @@
         <v>0.62999999999999989</v>
       </c>
       <c r="J55" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A55=A56),(SUMIFS(I:I, A:A, A55)+SUMIFS(D:D, A:A, A55))/SUMIFS(D:D, A:A, A55)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2553,7 +2635,7 @@
         <v>-1</v>
       </c>
       <c r="J56" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A56=A57),(SUMIFS(I:I, A:A, A56)+SUMIFS(D:D, A:A, A56))/SUMIFS(D:D, A:A, A56)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2588,7 +2670,7 @@
         <v>0.48</v>
       </c>
       <c r="J57" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A57=A58),(SUMIFS(I:I, A:A, A57)+SUMIFS(D:D, A:A, A57))/SUMIFS(D:D, A:A, A57)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2623,7 +2705,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J58" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A58=A59),(SUMIFS(I:I, A:A, A58)+SUMIFS(D:D, A:A, A58))/SUMIFS(D:D, A:A, A58)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2658,7 +2740,7 @@
         <v>0.48</v>
       </c>
       <c r="J59" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A59=A60),(SUMIFS(I:I, A:A, A59)+SUMIFS(D:D, A:A, A59))/SUMIFS(D:D, A:A, A59)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2693,7 +2775,7 @@
         <v>0.48</v>
       </c>
       <c r="J60" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A60=A61),(SUMIFS(I:I, A:A, A60)+SUMIFS(D:D, A:A, A60))/SUMIFS(D:D, A:A, A60)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2728,7 +2810,7 @@
         <v>-1</v>
       </c>
       <c r="J61" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A61=A62),(SUMIFS(I:I, A:A, A61)+SUMIFS(D:D, A:A, A61))/SUMIFS(D:D, A:A, A61)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2763,7 +2845,7 @@
         <v>0.5</v>
       </c>
       <c r="J62" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A62=A63),(SUMIFS(I:I, A:A, A62)+SUMIFS(D:D, A:A, A62))/SUMIFS(D:D, A:A, A62)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2798,7 +2880,7 @@
         <v>0.77</v>
       </c>
       <c r="J63" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A63=A64),(SUMIFS(I:I, A:A, A63)+SUMIFS(D:D, A:A, A63))/SUMIFS(D:D, A:A, A63)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2833,7 +2915,7 @@
         <v>-1</v>
       </c>
       <c r="J64" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A64=A65),(SUMIFS(I:I, A:A, A64)+SUMIFS(D:D, A:A, A64))/SUMIFS(D:D, A:A, A64)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2868,7 +2950,7 @@
         <v>0.62999999999999989</v>
       </c>
       <c r="J65" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A65=A66),(SUMIFS(I:I, A:A, A65)+SUMIFS(D:D, A:A, A65))/SUMIFS(D:D, A:A, A65)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2903,7 +2985,7 @@
         <v>-1</v>
       </c>
       <c r="J66" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A66=A67),(SUMIFS(I:I, A:A, A66)+SUMIFS(D:D, A:A, A66))/SUMIFS(D:D, A:A, A66)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2938,7 +3020,7 @@
         <v>0.8</v>
       </c>
       <c r="J67" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(NOT(A67=A68),(SUMIFS(I:I, A:A, A67)+SUMIFS(D:D, A:A, A67))/SUMIFS(D:D, A:A, A67)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -2968,12 +3050,12 @@
       <c r="H68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I68">
-        <f t="shared" ref="I68:I69" si="3">IF(H68="Yes",F68*D68-D68,-D68)</f>
+      <c r="I68" cm="1">
+        <f t="array" ref="I68">_xlfn.IFS(H68="Yes",F68*D68-D68,H68="no",-D68,H68="push",0)</f>
         <v>-1</v>
       </c>
       <c r="J68" s="2" t="str">
-        <f t="shared" ref="J68:J69" si="4">IF(NOT(A68=A69),(SUMIFS(I:I, A:A, A68)+SUMIFS(D:D, A:A, A68))/SUMIFS(D:D, A:A, A68)-1,"")</f>
+        <f>IF(NOT(A68=A69),(SUMIFS(I:I, A:A, A68)+SUMIFS(D:D, A:A, A68))/SUMIFS(D:D, A:A, A68)-1,"")</f>
         <v/>
       </c>
     </row>
@@ -3000,41 +3082,1417 @@
         <f t="shared" si="0"/>
         <v>0.18357487922705329</v>
       </c>
-      <c r="I69">
-        <f t="shared" si="3"/>
-        <v>-1</v>
+      <c r="H69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I69" cm="1">
+        <f t="array" ref="I69">_xlfn.IFS(H69="Yes",F69*D69-D69,H69="no",-D69,H69="push",0)</f>
+        <v>1.4500000000000002</v>
       </c>
       <c r="J69" s="2">
-        <f t="shared" si="4"/>
-        <v>0.17428571428571416</v>
+        <f>IF(NOT(A69=A70),(SUMIFS(I:I, A:A, A69)+SUMIFS(D:D, A:A, A69))/SUMIFS(D:D, A:A, A69)-1,"")</f>
+        <v>0.26178571428571429</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45392</v>
       </c>
+      <c r="B70" t="s">
+        <v>66</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>2.6</v>
+      </c>
+      <c r="F70">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G70" s="2">
+        <f t="shared" si="0"/>
+        <v>0.57692307692307665</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I70" cm="1">
+        <f t="array" ref="I70">_xlfn.IFS(H70="Yes",F70*D70-D70,H70="no",-D70,H70="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J70" s="2" t="str">
+        <f t="shared" ref="J70:J109" si="2">IF(NOT(A70=A71),(SUMIFS(I:I, A:A, A70)+SUMIFS(D:D, A:A, A70))/SUMIFS(D:D, A:A, A70)-1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B71" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1.3</v>
+      </c>
+      <c r="F71">
+        <v>1.69</v>
+      </c>
+      <c r="G71" s="2">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I71" cm="1">
+        <f t="array" ref="I71">_xlfn.IFS(H71="Yes",F71*D71-D71,H71="no",-D71,H71="push",0)</f>
+        <v>0.69</v>
+      </c>
+      <c r="J71" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B72" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F72">
+        <v>1.29</v>
+      </c>
+      <c r="G72" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13157894736842124</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" cm="1">
+        <f t="array" ref="I72">_xlfn.IFS(H72="Yes",F72*D72-D72,H72="no",-D72,H72="push",0)</f>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="J72" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B73" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1.6</v>
+      </c>
+      <c r="F73">
+        <v>2.15</v>
+      </c>
+      <c r="G73" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34374999999999978</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I73" cm="1">
+        <f t="array" ref="I73">_xlfn.IFS(H73="Yes",F73*D73-D73,H73="no",-D73,H73="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J73" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C74" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1.2</v>
+      </c>
+      <c r="F74">
+        <v>1.42</v>
+      </c>
+      <c r="G74" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18333333333333335</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I74" cm="1">
+        <f t="array" ref="I74">_xlfn.IFS(H74="Yes",F74*D74-D74,H74="no",-D74,H74="push",0)</f>
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="J74" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B75" t="s">
+        <v>69</v>
+      </c>
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G75" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27499999999999991</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I75" cm="1">
+        <f t="array" ref="I75">_xlfn.IFS(H75="Yes",F75*D75-D75,H75="no",-D75,H75="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J75" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B76" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1.2</v>
+      </c>
+      <c r="F76">
+        <v>1.45</v>
+      </c>
+      <c r="G76" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76" cm="1">
+        <f t="array" ref="I76">_xlfn.IFS(H76="Yes",F76*D76-D76,H76="no",-D76,H76="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J76" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1.17</v>
+      </c>
+      <c r="F77">
+        <v>1.42</v>
+      </c>
+      <c r="G77" s="2">
+        <f t="shared" ref="G77:G108" si="3">F77/E77-1</f>
+        <v>0.21367521367521358</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" cm="1">
+        <f t="array" ref="I77">_xlfn.IFS(H77="Yes",F77*D77-D77,H77="no",-D77,H77="push",0)</f>
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="J77" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B78" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1.28</v>
+      </c>
+      <c r="F78">
+        <v>1.59</v>
+      </c>
+      <c r="G78" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2421875</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" cm="1">
+        <f t="array" ref="I78">_xlfn.IFS(H78="Yes",F78*D78-D78,H78="no",-D78,H78="push",0)</f>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="J78" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B79" t="s">
+        <v>70</v>
+      </c>
+      <c r="C79" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>1.44</v>
+      </c>
+      <c r="F79">
+        <v>1.71</v>
+      </c>
+      <c r="G79" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1875</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79" cm="1">
+        <f t="array" ref="I79">_xlfn.IFS(H79="Yes",F79*D79-D79,H79="no",-D79,H79="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J79" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" t="s">
+        <v>25</v>
+      </c>
       <c r="D80">
-        <f>SUM(D2:D79)</f>
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>1.96</v>
+      </c>
+      <c r="F80">
+        <v>2.6</v>
+      </c>
+      <c r="G80" s="2">
+        <f t="shared" si="3"/>
+        <v>0.3265306122448981</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I80" cm="1">
+        <f t="array" ref="I80">_xlfn.IFS(H80="Yes",F80*D80-D80,H80="no",-D80,H80="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J80" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B81" t="s">
+        <v>57</v>
+      </c>
+      <c r="C81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>1.3</v>
+      </c>
+      <c r="F81">
+        <v>1.65</v>
+      </c>
+      <c r="G81" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26923076923076916</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" cm="1">
+        <f t="array" ref="I81">_xlfn.IFS(H81="Yes",F81*D81-D81,H81="no",-D81,H81="push",0)</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="J81" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B82" t="s">
         <v>73</v>
       </c>
-      <c r="I80">
-        <f>SUM(I2:I79)+D80</f>
-        <v>75.48</v>
-      </c>
-    </row>
-    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I81" s="3">
-        <f>I80/D80-1</f>
-        <v>3.3972602739726021E-2</v>
-      </c>
-      <c r="J81" t="s">
+      <c r="C82" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>1.59</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="G82" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25786163522012573</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I82" cm="1">
+        <f t="array" ref="I82">_xlfn.IFS(H82="Yes",F82*D82-D82,H82="no",-D82,H82="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J82" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83" t="s">
+        <v>56</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>1.59</v>
+      </c>
+      <c r="F83">
+        <v>2.15</v>
+      </c>
+      <c r="G83" s="2">
+        <f t="shared" si="3"/>
+        <v>0.35220125786163514</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I83" cm="1">
+        <f t="array" ref="I83">_xlfn.IFS(H83="Yes",F83*D83-D83,H83="no",-D83,H83="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J83" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B84" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F84">
+        <v>1.34</v>
+      </c>
+      <c r="G84" s="2">
+        <f t="shared" si="3"/>
+        <v>0.21818181818181825</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I84" cm="1">
+        <f t="array" ref="I84">_xlfn.IFS(H84="Yes",F84*D84-D84,H84="no",-D84,H84="push",0)</f>
+        <v>0</v>
+      </c>
+      <c r="J84" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>1.25</v>
+      </c>
+      <c r="F85">
+        <v>1.5</v>
+      </c>
+      <c r="G85" s="2">
+        <f t="shared" si="3"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I85" cm="1">
+        <f t="array" ref="I85">_xlfn.IFS(H85="Yes",F85*D85-D85,H85="no",-D85,H85="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J85" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B86" t="s">
+        <v>77</v>
+      </c>
+      <c r="C86" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86">
+        <v>1.77</v>
+      </c>
+      <c r="F86">
+        <v>2.1</v>
+      </c>
+      <c r="G86" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18644067796610164</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I86" cm="1">
+        <f t="array" ref="I86">_xlfn.IFS(H86="Yes",F86*D86-D86,H86="no",-D86,H86="push",0)</f>
+        <v>3.3000000000000007</v>
+      </c>
+      <c r="J86" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1.48</v>
+      </c>
+      <c r="F87">
+        <v>1.69</v>
+      </c>
+      <c r="G87" s="2">
+        <f t="shared" si="3"/>
+        <v>0.14189189189189189</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I87" cm="1">
+        <f t="array" ref="I87">_xlfn.IFS(H87="Yes",F87*D87-D87,H87="no",-D87,H87="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J87" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>56</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1.45</v>
+      </c>
+      <c r="F88">
+        <v>2.1</v>
+      </c>
+      <c r="G88" s="2">
+        <f t="shared" si="3"/>
+        <v>0.44827586206896552</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I88" cm="1">
+        <f t="array" ref="I88">_xlfn.IFS(H88="Yes",F88*D88-D88,H88="no",-D88,H88="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J88" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" t="s">
+        <v>56</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>1.52</v>
+      </c>
+      <c r="F89">
+        <v>2.75</v>
+      </c>
+      <c r="G89" s="2">
+        <f t="shared" si="3"/>
+        <v>0.80921052631578938</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I89" cm="1">
+        <f t="array" ref="I89">_xlfn.IFS(H89="Yes",F89*D89-D89,H89="no",-D89,H89="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J89" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B90" t="s">
+        <v>78</v>
+      </c>
+      <c r="C90" t="s">
+        <v>56</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>1.56</v>
+      </c>
+      <c r="F90">
+        <v>2.9</v>
+      </c>
+      <c r="G90" s="2">
+        <f t="shared" si="3"/>
+        <v>0.85897435897435881</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I90" cm="1">
+        <f t="array" ref="I90">_xlfn.IFS(H90="Yes",F90*D90-D90,H90="no",-D90,H90="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J90" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>1.45</v>
+      </c>
+      <c r="F91">
+        <v>1.67</v>
+      </c>
+      <c r="G91" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15172413793103456</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I91" cm="1">
+        <f t="array" ref="I91">_xlfn.IFS(H91="Yes",F91*D91-D91,H91="no",-D91,H91="push",0)</f>
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="J91" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B92" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" t="s">
+        <v>27</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>1.08</v>
+      </c>
+      <c r="F92">
+        <v>1.25</v>
+      </c>
+      <c r="G92" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15740740740740744</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I92" cm="1">
+        <f t="array" ref="I92">_xlfn.IFS(H92="Yes",F92*D92-D92,H92="no",-D92,H92="push",0)</f>
+        <v>0.25</v>
+      </c>
+      <c r="J92" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B93" t="s">
+        <v>79</v>
+      </c>
+      <c r="C93" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>3.3</v>
+      </c>
+      <c r="F93">
+        <v>4.5</v>
+      </c>
+      <c r="G93" s="2">
+        <f t="shared" si="3"/>
+        <v>0.36363636363636376</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I93" cm="1">
+        <f t="array" ref="I93">_xlfn.IFS(H93="Yes",F93*D93-D93,H93="no",-D93,H93="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J93" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B94" t="s">
+        <v>62</v>
+      </c>
+      <c r="C94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1.24</v>
+      </c>
+      <c r="F94">
+        <v>1.42</v>
+      </c>
+      <c r="G94" s="2">
+        <f t="shared" si="3"/>
+        <v>0.14516129032258052</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I94" cm="1">
+        <f t="array" ref="I94">_xlfn.IFS(H94="Yes",F94*D94-D94,H94="no",-D94,H94="push",0)</f>
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="J94" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B95" t="s">
+        <v>80</v>
+      </c>
+      <c r="C95" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>1.36</v>
+      </c>
+      <c r="F95">
+        <v>1.61</v>
+      </c>
+      <c r="G95" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18382352941176472</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" cm="1">
+        <f t="array" ref="I95">_xlfn.IFS(H95="Yes",F95*D95-D95,H95="no",-D95,H95="push",0)</f>
+        <v>0.6100000000000001</v>
+      </c>
+      <c r="J95" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B96" t="s">
+        <v>81</v>
+      </c>
+      <c r="C96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>1.73</v>
+      </c>
+      <c r="F96">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G96" s="2">
+        <f t="shared" si="3"/>
+        <v>0.32947976878612706</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I96" cm="1">
+        <f t="array" ref="I96">_xlfn.IFS(H96="Yes",F96*D96-D96,H96="no",-D96,H96="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J96" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B97" t="s">
+        <v>82</v>
+      </c>
+      <c r="C97" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>3.06</v>
+      </c>
+      <c r="F97">
+        <v>3.8</v>
+      </c>
+      <c r="G97" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24183006535947715</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I97" cm="1">
+        <f t="array" ref="I97">_xlfn.IFS(H97="Yes",F97*D97-D97,H97="no",-D97,H97="push",0)</f>
+        <v>2.8</v>
+      </c>
+      <c r="J97" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B98" t="s">
+        <v>83</v>
+      </c>
+      <c r="C98" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>3.61</v>
+      </c>
+      <c r="F98">
+        <v>6.5</v>
+      </c>
+      <c r="G98" s="2">
+        <f t="shared" si="3"/>
+        <v>0.80055401662049874</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I98" cm="1">
+        <f t="array" ref="I98">_xlfn.IFS(H98="Yes",F98*D98-D98,H98="no",-D98,H98="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J98" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B99" t="s">
+        <v>62</v>
+      </c>
+      <c r="C99" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1.24</v>
+      </c>
+      <c r="F99">
+        <v>1.61</v>
+      </c>
+      <c r="G99" s="2">
+        <f t="shared" si="3"/>
+        <v>0.29838709677419373</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I99" cm="1">
+        <f t="array" ref="I99">_xlfn.IFS(H99="Yes",F99*D99-D99,H99="no",-D99,H99="push",0)</f>
+        <v>0.6100000000000001</v>
+      </c>
+      <c r="J99" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B100" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" t="s">
+        <v>56</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>1.34</v>
+      </c>
+      <c r="F100">
+        <v>1.67</v>
+      </c>
+      <c r="G100" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24626865671641784</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I100" cm="1">
+        <f t="array" ref="I100">_xlfn.IFS(H100="Yes",F100*D100-D100,H100="no",-D100,H100="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J100" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B101" t="s">
+        <v>62</v>
+      </c>
+      <c r="C101" t="s">
+        <v>27</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>1.54</v>
+      </c>
+      <c r="F101">
+        <v>2.25</v>
+      </c>
+      <c r="G101" s="2">
+        <f t="shared" si="3"/>
+        <v>0.46103896103896091</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I101" cm="1">
+        <f t="array" ref="I101">_xlfn.IFS(H101="Yes",F101*D101-D101,H101="no",-D101,H101="push",0)</f>
+        <v>1.25</v>
+      </c>
+      <c r="J101" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B102" t="s">
+        <v>48</v>
+      </c>
+      <c r="C102" t="s">
+        <v>56</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>1.39</v>
+      </c>
+      <c r="F102">
+        <v>1.83</v>
+      </c>
+      <c r="G102" s="2">
+        <f t="shared" si="3"/>
+        <v>0.31654676258992831</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I102" cm="1">
+        <f t="array" ref="I102">_xlfn.IFS(H102="Yes",F102*D102-D102,H102="no",-D102,H102="push",0)</f>
+        <v>0.83000000000000007</v>
+      </c>
+      <c r="J102" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B103" t="s">
+        <v>84</v>
+      </c>
+      <c r="C103" t="s">
+        <v>27</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>1.23</v>
+      </c>
+      <c r="F103">
+        <v>1.54</v>
+      </c>
+      <c r="G103" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2520325203252034</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I103" cm="1">
+        <f t="array" ref="I103">_xlfn.IFS(H103="Yes",F103*D103-D103,H103="no",-D103,H103="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J103" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C104" t="s">
+        <v>27</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>1.21</v>
+      </c>
+      <c r="F104">
+        <v>1.57</v>
+      </c>
+      <c r="G104" s="2">
+        <f t="shared" si="3"/>
+        <v>0.29752066115702491</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" cm="1">
+        <f t="array" ref="I104">_xlfn.IFS(H104="Yes",F104*D104-D104,H104="no",-D104,H104="push",0)</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="J104" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B105" t="s">
+        <v>50</v>
+      </c>
+      <c r="C105" t="s">
+        <v>27</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>1.49</v>
+      </c>
+      <c r="F105">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="G105" s="2">
+        <f t="shared" si="3"/>
+        <v>0.37583892617449655</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105" cm="1">
+        <f t="array" ref="I105">_xlfn.IFS(H105="Yes",F105*D105-D105,H105="no",-D105,H105="push",0)</f>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="J105" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B106" t="s">
+        <v>49</v>
+      </c>
+      <c r="C106" t="s">
+        <v>19</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>1.31</v>
+      </c>
+      <c r="F106">
+        <v>1.51</v>
+      </c>
+      <c r="G106" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15267175572519087</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I106" cm="1">
+        <f t="array" ref="I106">_xlfn.IFS(H106="Yes",F106*D106-D106,H106="no",-D106,H106="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J106" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B107" t="s">
+        <v>51</v>
+      </c>
+      <c r="C107" t="s">
+        <v>19</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>1.47</v>
+      </c>
+      <c r="F107">
+        <v>1.71</v>
+      </c>
+      <c r="G107" s="2">
+        <f t="shared" si="3"/>
+        <v>0.16326530612244894</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I107" cm="1">
+        <f t="array" ref="I107">_xlfn.IFS(H107="Yes",F107*D107-D107,H107="no",-D107,H107="push",0)</f>
+        <v>0.71</v>
+      </c>
+      <c r="J107" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B108" t="s">
+        <v>50</v>
+      </c>
+      <c r="C108" t="s">
+        <v>19</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F108">
+        <v>3.3</v>
+      </c>
+      <c r="G108" s="2">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999978</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I108" cm="1">
+        <f t="array" ref="I108">_xlfn.IFS(H108="Yes",F108*D108-D108,H108="no",-D108,H108="push",0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J108" s="2">
+        <f t="shared" si="2"/>
+        <v>-9.4390243902438997E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>45393</v>
+      </c>
+      <c r="I109" t="e" cm="1">
+        <f t="array" ref="I109">_xlfn.IFS(H109="Yes",F109*D109-D109,H109="no",-D109,H109="push",0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J109" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="133" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <f>SUM(D2:D101)</f>
+        <v>107</v>
+      </c>
+      <c r="I133">
+        <f>SUM(I2:I99)+D133</f>
+        <v>107.65</v>
+      </c>
+    </row>
+    <row r="134" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="I134" s="3">
+        <f>I133/D133-1</f>
+        <v>6.0747663551401487E-3</v>
+      </c>
+      <c r="J134" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I109" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
name update for old version
</commit_message>
<xml_diff>
--- a/Bet Stamps.xlsx
+++ b/Bet Stamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsham\.spyder-py3\beating-the-books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0D26FD-6BFE-4C54-A175-D8CD9AE167A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97FEF55-2870-495F-8BE2-460AFC4219BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3990" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15509,7 +15509,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Results Cleanup and runtime optimzed
bets also published
</commit_message>
<xml_diff>
--- a/Bet Stamps.xlsx
+++ b/Bet Stamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsham\.spyder-py3\beating-the-books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2E9B8D-5C7D-47CD-80D6-FADC1B8D1139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84A29F-AA0B-48F1-8519-4DE1EBB5B548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="5032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5499" uniqueCount="5032">
   <si>
     <t>Date</t>
   </si>
@@ -15527,7 +15527,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16124,6 +16124,9 @@
         <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
+      <c r="H17" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I17">
         <f t="shared" si="1"/>
         <v>-1</v>
@@ -16156,6 +16159,9 @@
         <f t="shared" si="0"/>
         <v>0.37209302325581395</v>
       </c>
+      <c r="H18" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I18">
         <f t="shared" si="1"/>
         <v>-1</v>
@@ -16188,6 +16194,9 @@
         <f t="shared" si="0"/>
         <v>1.5714285714285716</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I19">
         <f t="shared" si="1"/>
         <v>-1</v>
@@ -16220,6 +16229,9 @@
         <f t="shared" si="0"/>
         <v>0.90647482014388503</v>
       </c>
+      <c r="H20" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I20">
         <f t="shared" si="1"/>
         <v>-1</v>
@@ -16252,9 +16264,12 @@
         <f t="shared" si="0"/>
         <v>0.83333333333333348</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="I21">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.87000000000000011</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="3"/>
@@ -16284,6 +16299,9 @@
         <f t="shared" si="0"/>
         <v>1.0866141732283463</v>
       </c>
+      <c r="H22" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I22">
         <f t="shared" si="1"/>
         <v>-1</v>
@@ -16316,13 +16334,16 @@
         <f t="shared" si="0"/>
         <v>0.85000000000000009</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="I23">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>2.7</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-0.20428571428571429</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -18777,13 +18798,13 @@
       </c>
       <c r="I189">
         <f>SUM(I2:I188)+D189</f>
-        <v>23.95</v>
+        <v>29.52</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I190" s="3">
         <f>I189/D189-1</f>
-        <v>8.8636363636363624E-2</v>
+        <v>0.3418181818181818</v>
       </c>
       <c r="J190" t="s">
         <v>26</v>

</xml_diff>